<commit_message>
subi wbs en UNIVERSIDAD TECNOLÓGICA NACIONAL.docx
</commit_message>
<xml_diff>
--- a/Proyecto final/BenefictsYFeatures.xlsx
+++ b/Proyecto final/BenefictsYFeatures.xlsx
@@ -30,9 +30,6 @@
     <t>Status (%)</t>
   </si>
   <si>
-    <t>Captura de imagenes y procesamiento inicial de inagenes</t>
-  </si>
-  <si>
     <t>Captura eficiente de imagenes permite realizar una entrada eficiente para el procesamiento.</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Manejo de video sampling y deteccion de movimientos de video</t>
   </si>
   <si>
-    <t>Combinar la interaccion de video con acciones de vision</t>
-  </si>
-  <si>
     <t>Al poder combinar la interraccion de video con el procesamiento y clasificacion</t>
   </si>
   <si>
@@ -115,6 +109,12 @@
   </si>
   <si>
     <t>según su informacion que uso se le va dar</t>
+  </si>
+  <si>
+    <t>Captura de imagenes y procesamiento inicial de imagenes</t>
+  </si>
+  <si>
+    <t>relacion entre la interaccion de video con acciones de vision</t>
   </si>
 </sst>
 </file>
@@ -457,13 +457,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK27"/>
+  <dimension ref="A1:AMK26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="1"/>
     <col min="2" max="2" width="47.5703125" style="1"/>
@@ -471,7 +471,7 @@
     <col min="4" max="1025" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,188 +490,180 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="F2" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="12.75">
+    <row r="3" spans="1:6">
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.75">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="12.75">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="12.75"/>
-    <row r="9" spans="1:6" ht="12.75">
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12.75">
+    <row r="10" spans="1:6">
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="12.75"/>
-    <row r="12" spans="1:6" ht="12.75">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="12.75">
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="12.75"/>
-    <row r="15" spans="1:6" ht="12.75">
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="12.75">
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="12.75"/>
-    <row r="18" spans="1:6" ht="12.75">
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="12.75"/>
-    <row r="20" spans="1:6" ht="12.75">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="12.75">
-      <c r="C21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="12.75"/>
-    <row r="23" spans="1:6" ht="12.75">
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="C24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="12.75">
-      <c r="C24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="12.75"/>
-    <row r="26" spans="1:6" ht="12.75">
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="12.75"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
@@ -688,7 +680,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1025" width="10.5703125" style="1"/>
   </cols>
@@ -708,7 +700,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1025" width="10.5703125" style="1"/>
   </cols>

</xml_diff>